<commit_message>
Update to focus on data science jobs
</commit_message>
<xml_diff>
--- a/1_Spreadsheets_Intro/2_Workbooks/1_Workbooks_Overview.xlsx
+++ b/1_Spreadsheets_Intro/2_Workbooks/1_Workbooks_Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaderPC\Documents\GitHub\Excel_Data_Analytics_Course\1_Spreadsheets_Intro\2_Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70700CF-A28A-425F-B068-026A2BD36093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7452BC34-58F9-4E03-9C4A-A7FD8B3FA007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0854EC15-9DEA-44B3-92B4-E32714D02E5C}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Month</t>
   </si>
   <si>
-    <t>Sales</t>
-  </si>
-  <si>
     <t>January</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>March</t>
+  </si>
+  <si>
+    <t>Job Postings</t>
   </si>
 </sst>
 </file>
@@ -425,41 +425,44 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>51000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>74000</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>64000</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>